<commit_message>
Préparation à la distribution du noyau
</commit_message>
<xml_diff>
--- a/Docs/projet/Altaïr-Tests de charge.xlsx
+++ b/Docs/projet/Altaïr-Tests de charge.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
   <si>
     <t xml:space="preserve">LOGICIEL  ALTAÏR – EXTRACTION DES DONNEES DE PAYE </t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Ile-de-France (Paris)</t>
+  </si>
+  <si>
+    <t>IDF*</t>
+  </si>
+  <si>
+    <t>Ile-de-France sur PC propre</t>
   </si>
 </sst>
 </file>
@@ -419,19 +425,6 @@
             <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Feuille1!$C$13:$C$44</c:f>
@@ -502,7 +495,7 @@
                   <c:v>938214</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10108198</c:v>
+                  <c:v>34953667</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>670046</c:v>
@@ -607,7 +600,7 @@
                   <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>116</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>178</c:v>
@@ -652,13 +645,16 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85107072"/>
-        <c:axId val="85108992"/>
+        <c:axId val="85635840"/>
+        <c:axId val="85637760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85107072"/>
+        <c:axId val="85635840"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:max val="100000000"/>
+          <c:min val="10000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -732,12 +728,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85108992"/>
+        <c:crossAx val="85637760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85108992"/>
+        <c:axId val="85637760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +809,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85107072"/>
+        <c:crossAx val="85635840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -868,16 +864,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1125360</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>525600</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>66600</xdr:rowOff>
+      <xdr:colOff>525599</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1186,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1668,19 +1664,19 @@
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" s="18"/>
       <c r="C34" s="9">
-        <v>10108198</v>
+        <v>34953667</v>
       </c>
       <c r="D34" s="9">
-        <v>369145</v>
+        <v>1369862</v>
       </c>
       <c r="E34" s="9">
-        <v>86582</v>
+        <v>224360</v>
       </c>
       <c r="F34" s="9">
-        <v>116</v>
+        <v>155</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
@@ -1877,19 +1873,19 @@
       </c>
       <c r="C46" s="13">
         <f>SUM(C13:C45)</f>
-        <v>50115529</v>
+        <v>74960998</v>
       </c>
       <c r="D46" s="13">
         <f>SUM(D13:D45)</f>
-        <v>2147633</v>
+        <v>3148350</v>
       </c>
       <c r="E46" s="13">
         <f>SUM(E13:E45)</f>
-        <v>423130</v>
+        <v>560908</v>
       </c>
       <c r="F46" s="13">
         <f>C46/E46</f>
-        <v>118.44002788741049</v>
+        <v>133.64223366398767</v>
       </c>
       <c r="G46" s="14"/>
     </row>
@@ -1926,6 +1922,14 @@
       </c>
       <c r="H51" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>